<commit_message>
16/10/23 - push 1
</commit_message>
<xml_diff>
--- a/sop/aula 6/Pasta2.xlsx
+++ b/sop/aula 6/Pasta2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\senai\sop\aula 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Guilherme Carvalho\senai\sop\aula 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095337A3-E6AD-492F-8A19-753A2AEF7B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C733BFBC-0755-439F-B898-EE918B6D73A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{48C18CA6-12A2-41EB-9BDC-A7A790894FB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{48C18CA6-12A2-41EB-9BDC-A7A790894FB1}"/>
   </bookViews>
   <sheets>
     <sheet name="exercício 2" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
   <si>
     <t>nome</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>se e(genero, idade, dias); apto; se(e(genero, idade, dias);apto; inapto)</t>
+  </si>
+  <si>
+    <t>sal. Liquido</t>
   </si>
 </sst>
 </file>
@@ -216,7 +219,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,13 +242,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -257,11 +278,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -283,8 +306,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="40% - Ênfase6" xfId="3" builtinId="51"/>
+    <cellStyle name="Bom" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -891,32 +924,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FD8761-B4D8-48BB-A370-301DC5172586}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="5" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -928,84 +967,95 @@
       <c r="E2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="12">
         <v>1000</v>
       </c>
       <c r="C3" s="4">
-        <f>IF(B3&lt;1100,B3*$H$3,IF(B3&lt;2203.48,B3*$H$4,IF(B3&lt;3305.22,B3*$H$5,B3*$H$6)))</f>
+        <f>IF(B3&lt;1100,B3*$I$3,IF(B3&lt;2203.48,B3*$I$4,IF(B3&lt;3305.22,B3*$I$5,B3*$I$6)))</f>
         <v>75</v>
       </c>
       <c r="D3" s="4">
         <f>B3-C3</f>
         <v>925</v>
       </c>
-      <c r="E3" s="8" t="str">
-        <f>IF(D3&lt;=2112,"isento",IF(D3&lt;=2826.65,D3*$K$4,IF(D3&lt;=3751.05,D3*$K$5,IF(D3&lt;=4664.68,D3*$K$6,D3*$K$7))))</f>
-        <v>isento</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E3" s="8">
+        <f>IF(D3&lt;=2112,0,IF(D3&lt;=2826.65,D3*$L$4,IF(D3&lt;=3751.05,D3*$L$5,IF(D3&lt;=4664.68,D3*$L$6,D3*$L$7))))</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3-E3</f>
+        <v>925</v>
+      </c>
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="7">
+      <c r="L3" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="12">
         <v>2000</v>
       </c>
       <c r="C4" s="4">
-        <f t="shared" ref="C4:C11" si="0">IF(B4&lt;1100,B4*$H$3,IF(B4&lt;2203.48,B4*$H$4,IF(B4&lt;3305.22,B4*$H$5,B4*$H$6)))</f>
+        <f t="shared" ref="C4:C11" si="0">IF(B4&lt;1100,B4*$I$3,IF(B4&lt;2203.48,B4*$I$4,IF(B4&lt;3305.22,B4*$I$5,B4*$I$6)))</f>
         <v>180</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" ref="D4:D11" si="1">B4-C4</f>
         <v>1820</v>
       </c>
-      <c r="E4" s="8" t="str">
-        <f t="shared" ref="E4:E11" si="2">IF(D4&lt;=2112,"isento",IF(D4&lt;=2826.65,D4*$K$4,IF(D4&lt;=3751.05,D4*$K$5,IF(D4&lt;=4664.68,D4*$K$6,D4*$K$7))))</f>
-        <v>isento</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E4" s="8">
+        <f t="shared" ref="E4:E11" si="2">IF(D4&lt;=2112,0,IF(D4&lt;=2826.65,D4*$L$4,IF(D4&lt;=3751.05,D4*$L$5,IF(D4&lt;=4664.68,D4*$L$6,D4*$L$7))))</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" ref="F4:F11" si="3">D4-E4</f>
+        <v>1820</v>
+      </c>
+      <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="7">
         <v>0.09</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="6">
+      <c r="L4" s="6">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="12">
         <v>3000</v>
       </c>
       <c r="C5" s="4">
@@ -1016,29 +1066,33 @@
         <f t="shared" si="1"/>
         <v>2640</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="8">
         <f t="shared" si="2"/>
         <v>198</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="8">
+        <f t="shared" si="3"/>
+        <v>2442</v>
+      </c>
+      <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>0.12</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" t="s">
+      <c r="J5" s="5"/>
+      <c r="K5" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="7">
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="12">
         <v>4000</v>
       </c>
       <c r="C6" s="4">
@@ -1049,29 +1103,33 @@
         <f t="shared" si="1"/>
         <v>3440</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="8">
         <f t="shared" si="2"/>
         <v>516</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" s="8">
+        <f t="shared" si="3"/>
+        <v>2924</v>
+      </c>
+      <c r="H6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="6">
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="12">
         <v>5000</v>
       </c>
       <c r="C7" s="4">
@@ -1082,22 +1140,26 @@
         <f t="shared" si="1"/>
         <v>4300</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="8">
         <f t="shared" si="2"/>
         <v>967.5</v>
       </c>
-      <c r="J7" t="s">
+      <c r="F7" s="8">
+        <f t="shared" si="3"/>
+        <v>3332.5</v>
+      </c>
+      <c r="K7" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="6">
+      <c r="L7" s="6">
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="12">
         <v>6000</v>
       </c>
       <c r="C8" s="4">
@@ -1108,16 +1170,20 @@
         <f t="shared" si="1"/>
         <v>5160</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="8">
         <f t="shared" si="2"/>
         <v>1419.0000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F8" s="8">
+        <f t="shared" si="3"/>
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="12">
         <v>7000</v>
       </c>
       <c r="C9" s="4">
@@ -1128,16 +1194,20 @@
         <f t="shared" si="1"/>
         <v>6020</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="8">
         <f t="shared" si="2"/>
         <v>1655.5000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9" s="8">
+        <f t="shared" si="3"/>
+        <v>4364.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="12">
         <v>8000</v>
       </c>
       <c r="C10" s="4">
@@ -1148,16 +1218,20 @@
         <f t="shared" si="1"/>
         <v>6880</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="8">
         <f t="shared" si="2"/>
         <v>1892.0000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="F10" s="8">
+        <f t="shared" si="3"/>
+        <v>4988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="12">
         <v>10000</v>
       </c>
       <c r="C11" s="4">
@@ -1168,12 +1242,19 @@
         <f t="shared" si="1"/>
         <v>8600</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="8">
         <f t="shared" si="2"/>
         <v>2365</v>
       </c>
+      <c r="F11" s="8">
+        <f t="shared" si="3"/>
+        <v>6235</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>